<commit_message>
the new tests stats
</commit_message>
<xml_diff>
--- a/Reports/3.0.0-2020_05_06.xlsx
+++ b/Reports/3.0.0-2020_05_06.xlsx
@@ -8,21 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\VirtoCommerce\vc-benchmark\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B168EE8-0BFF-4C6C-A8F8-041EA8840C63}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF001BA6-C74D-4053-A9BE-28E0D381D179}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test enviroment" sheetId="12" r:id="rId1"/>
-    <sheet name="Mixed test data" sheetId="14" r:id="rId2"/>
+    <sheet name="Mixed test data for graph" sheetId="14" r:id="rId2"/>
     <sheet name="3.0.0 - 2020-06-05" sheetId="10" r:id="rId3"/>
-    <sheet name="Charts" sheetId="13" r:id="rId4"/>
+    <sheet name="2.13.63 - 2020-06-05" sheetId="15" r:id="rId4"/>
+    <sheet name="Charts" sheetId="13" r:id="rId5"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="1" hidden="1">'Mixed test data'!$A$1:$D$12</definedName>
+    <definedName name="ExternalData_1" localSheetId="1" hidden="1">'Mixed test data for graph'!$A$1:$D$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="73">
   <si>
     <t>Products</t>
   </si>
@@ -63,9 +61,6 @@
   </si>
   <si>
     <t>Lucene</t>
-  </si>
-  <si>
-    <t>Avg response time (sec)</t>
   </si>
   <si>
     <t>Load pattern</t>
@@ -145,9 +140,6 @@
     <t>Caching:CacheSlidingExpiration</t>
   </si>
   <si>
-    <t xml:space="preserve">Full indexation time </t>
-  </si>
-  <si>
     <t>Scenarios</t>
   </si>
   <si>
@@ -268,9 +260,6 @@
     <t xml:space="preserve">Indexed search  prodcuts in the categories </t>
   </si>
   <si>
-    <t>5min</t>
-  </si>
-  <si>
     <t>Elapsed Time</t>
   </si>
   <si>
@@ -281,6 +270,15 @@
   </si>
   <si>
     <t>Avg. Resp Time</t>
+  </si>
+  <si>
+    <t>Platform restart time (sec)</t>
+  </si>
+  <si>
+    <t>Full indexation time (sec)</t>
+  </si>
+  <si>
+    <t>Avg response time (msec)</t>
   </si>
 </sst>
 </file>
@@ -354,18 +352,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -491,19 +489,19 @@
             <c:numRef>
               <c:f>'3.0.0 - 2020-06-05'!$C$3:$C$8</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>65</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60.6</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27.8</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>12</c:v>
@@ -524,7 +522,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Avg response time (sec)</c:v>
+            <c:v>Avg response time (ms)</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
@@ -553,25 +551,25 @@
             <c:numRef>
               <c:f>'3.0.0 - 2020-06-05'!$D$3:$D$8</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>1.58</c:v>
+                <c:pt idx="0">
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.75</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.68</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1599999999999999</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>350</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0499999999999998</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -741,7 +739,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -785,7 +783,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="t"/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -895,7 +893,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Mixed test data'!$B$1</c:f>
+              <c:f>'Mixed test data for graph'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -988,7 +986,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'Mixed test data'!$A$2:$A$12</c:f>
+              <c:f>'Mixed test data for graph'!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1030,7 +1028,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Mixed test data'!$B$2:$B$12</c:f>
+              <c:f>'Mixed test data for graph'!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1082,7 +1080,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Mixed test data'!$C$1</c:f>
+              <c:f>'Mixed test data for graph'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1175,7 +1173,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'Mixed test data'!$A$2:$A$12</c:f>
+              <c:f>'Mixed test data for graph'!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1217,7 +1215,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Mixed test data'!$C$2:$C$12</c:f>
+              <c:f>'Mixed test data for graph'!$C$2:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1285,7 +1283,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Mixed test data'!$D$1</c:f>
+              <c:f>'Mixed test data for graph'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1378,7 +1376,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'Mixed test data'!$A$2:$A$12</c:f>
+              <c:f>'Mixed test data for graph'!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1420,7 +1418,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Mixed test data'!$D$2:$D$12</c:f>
+              <c:f>'Mixed test data for graph'!$D$2:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1657,7 +1655,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="t"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1713,6 +1711,326 @@
     </a:ln>
     <a:effectLst/>
   </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Maintenability</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> tests </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.9612688384740609E-2"/>
+          <c:y val="0.10480659018746252"/>
+          <c:w val="0.78616780010580467"/>
+          <c:h val="0.84190568875519778"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'3.0.0 - 2020-06-05'!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Full indexation time (sec)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'3.0.0 - 2020-06-05'!$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-3EDD-4D75-B2C7-4E9E1819821E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'3.0.0 - 2020-06-05'!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Platform restart time (sec)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'3.0.0 - 2020-06-05'!$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-3EDD-4D75-B2C7-4E9E1819821E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1534818608"/>
+        <c:axId val="1486713888"/>
+        <c:extLst/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1534818608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1486713888"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1486713888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1534818608"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
   <c:txPr>
     <a:bodyPr/>
     <a:lstStyle/>
@@ -2316,16 +2634,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2350,131 +2668,45 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>438151</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Диаграмма 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CEB76D9-D175-4012-85A6-BA9B106C947E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Report 2019 Benchmark (comp)"/>
-      <sheetName val="Report 2019 Benchmark"/>
-      <sheetName val="2.13.63 - 2020 Baseline"/>
-      <sheetName val="3.0.0 - 2020 Baseline"/>
-      <sheetName val="3.0.0-rc - 2019 Baseline"/>
-      <sheetName val="2.13.49 - 2019 Baseline"/>
-      <sheetName val="Report 2017"/>
-      <sheetName val="B2 -2017"/>
-      <sheetName val="B3 - 2017"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5">
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>Category browsing</v>
-          </cell>
-          <cell r="D3">
-            <v>46.6</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>Product details page browsing</v>
-          </cell>
-          <cell r="D4">
-            <v>78.53</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>Search by unique search phrase</v>
-          </cell>
-          <cell r="D5">
-            <v>125</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v xml:space="preserve">Add product to cart </v>
-          </cell>
-          <cell r="D6">
-            <v>6.46</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>Mixed (category browsing 30%, product details 40%, Add product to cart 10%, Search by phrase 20%)</v>
-          </cell>
-          <cell r="D7">
-            <v>23.5</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>Return products by category 
-GET api/catalog/search/products</v>
-          </cell>
-          <cell r="D11">
-            <v>50</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12" t="str">
-            <v xml:space="preserve">Return product data by id 
-GET api/catalog/products/{id} </v>
-          </cell>
-          <cell r="D12">
-            <v>150</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13" t="str">
-            <v>Evaluate prices
-POST api/pricing/evaluate</v>
-          </cell>
-          <cell r="D13">
-            <v>78</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14" t="str">
-            <v>Save shopping cart
-POST api/cart</v>
-          </cell>
-          <cell r="D14">
-            <v>20.420000000000002</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15" t="str">
-            <v>Create order
-POST api/order</v>
-          </cell>
-          <cell r="D15">
-            <v>7</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16" t="str">
-            <v>Mixed
-category 30%, product 40%, pricing 10%,save cart 20%</v>
-          </cell>
-          <cell r="D16">
-            <v>78.05</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2768,8 +3000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD62DA76-516D-414D-98FD-2FD438DDFE1A}">
   <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56:B60"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2779,47 +3011,47 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2832,7 +3064,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11">
         <v>7854</v>
@@ -2848,7 +3080,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13">
         <v>344461</v>
@@ -2856,7 +3088,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14">
         <v>37745</v>
@@ -2864,7 +3096,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15">
         <v>20</v>
@@ -2877,7 +3109,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
         <v>4</v>
@@ -2885,15 +3117,15 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="9">
+        <v>25</v>
+      </c>
+      <c r="B19" s="8">
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
         <v>3</v>
@@ -2901,12 +3133,12 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B22">
         <v>300</v>
@@ -2914,7 +3146,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -2922,7 +3154,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B24">
         <v>10</v>
@@ -2930,7 +3162,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B25">
         <v>20</v>
@@ -2938,33 +3170,33 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B30">
         <v>20</v>
@@ -2972,15 +3204,15 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B32">
         <v>704</v>
@@ -2988,44 +3220,44 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" t="s">
         <v>60</v>
-      </c>
-      <c r="B35" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>31</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>38</v>
+        <v>29</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B37" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B38">
         <v>1372</v>
@@ -3033,70 +3265,70 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B39" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B41" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B43" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B44" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B46" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>44</v>
-      </c>
-      <c r="B47" s="10" t="s">
-        <v>37</v>
+        <v>42</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B48">
         <v>1372</v>
@@ -3104,20 +3336,20 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B50" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B51">
         <v>7</v>
@@ -3125,7 +3357,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -3133,7 +3365,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -3141,7 +3373,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -3149,46 +3381,46 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B56" s="11">
+        <v>28</v>
+      </c>
+      <c r="B56" s="10">
         <v>0.3</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B57" s="11">
+        <v>34</v>
+      </c>
+      <c r="B57" s="10">
         <v>0.4</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B58" s="11">
+        <v>40</v>
+      </c>
+      <c r="B58" s="10">
         <v>0.15</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B59" s="11">
+        <v>44</v>
+      </c>
+      <c r="B59" s="10">
         <v>0.1</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B60" s="11">
+        <v>50</v>
+      </c>
+      <c r="B60" s="10">
         <v>0.05</v>
       </c>
     </row>
@@ -3216,20 +3448,20 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" t="s">
         <v>69</v>
       </c>
-      <c r="B1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" t="s">
-        <v>72</v>
-      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="14">
+      <c r="A2" s="12">
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="B2" s="2">
@@ -3243,7 +3475,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="14">
+      <c r="A3" s="12">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="B3" s="2">
@@ -3257,7 +3489,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="14">
+      <c r="A4" s="12">
         <v>3.125E-2</v>
       </c>
       <c r="B4" s="2">
@@ -3271,7 +3503,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="14">
+      <c r="A5" s="12">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="B5" s="2">
@@ -3285,7 +3517,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="14">
+      <c r="A6" s="12">
         <v>5.2083333333333336E-2</v>
       </c>
       <c r="B6" s="2">
@@ -3299,7 +3531,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="14">
+      <c r="A7" s="12">
         <v>6.25E-2</v>
       </c>
       <c r="B7" s="2">
@@ -3313,7 +3545,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="14">
+      <c r="A8" s="12">
         <v>7.2916666666666671E-2</v>
       </c>
       <c r="B8" s="2">
@@ -3327,7 +3559,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="14">
+      <c r="A9" s="12">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="B9" s="2">
@@ -3341,7 +3573,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="14">
+      <c r="A10" s="12">
         <v>9.375E-2</v>
       </c>
       <c r="B10" s="2">
@@ -3355,7 +3587,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
+      <c r="A11" s="12">
         <v>0.10416666666666667</v>
       </c>
       <c r="B11" s="2">
@@ -3369,7 +3601,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="14">
+      <c r="A12" s="12">
         <v>0.11458333333333333</v>
       </c>
       <c r="B12" s="2">
@@ -3392,10 +3624,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDEACA4-D9DD-47D9-852C-381272874DE7}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3404,12 +3636,12 @@
     <col min="2" max="2" width="8.5703125" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" customWidth="1"/>
     <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -3420,24 +3652,24 @@
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="12">
-        <v>35</v>
-      </c>
-      <c r="D3" s="7">
-        <v>1.58</v>
+        <v>65</v>
+      </c>
+      <c r="C3" s="15">
+        <v>36</v>
+      </c>
+      <c r="D3" s="15">
+        <v>130</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="6">
@@ -3446,13 +3678,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="2">
-        <v>65</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1.75</v>
+        <v>34</v>
+      </c>
+      <c r="C4" s="6">
+        <v>55</v>
+      </c>
+      <c r="D4" s="6">
+        <v>80</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="6">
@@ -3461,13 +3693,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="2">
-        <v>60.6</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1.68</v>
+        <v>63</v>
+      </c>
+      <c r="C5" s="6">
+        <v>49</v>
+      </c>
+      <c r="D5" s="6">
+        <v>98</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="6">
@@ -3475,14 +3707,14 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="2">
-        <v>27.8</v>
-      </c>
-      <c r="D6" s="2">
-        <v>1.1599999999999999</v>
+      <c r="A6" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="6">
+        <v>32</v>
+      </c>
+      <c r="D6" s="6">
+        <v>140</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="6">
@@ -3491,28 +3723,28 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="2">
+        <v>45</v>
+      </c>
+      <c r="C7" s="6">
         <v>12</v>
       </c>
-      <c r="D7" s="2">
-        <v>2</v>
+      <c r="D7" s="6">
+        <v>350</v>
       </c>
       <c r="F7" s="6">
         <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="2">
+      <c r="A8" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="6">
         <v>24.1</v>
       </c>
-      <c r="D8" s="2">
-        <v>2.0499999999999998</v>
+      <c r="D8" s="6">
+        <v>200</v>
       </c>
       <c r="F8" s="6">
         <v>70</v>
@@ -3520,12 +3752,20 @@
     </row>
     <row r="9" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>68</v>
+        <v>71</v>
+      </c>
+      <c r="C9" s="14">
+        <v>300</v>
       </c>
       <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="6">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3537,11 +3777,164 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2476426-BE5C-4232-90B2-8638C3644BEA}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="6">
+        <v>37</v>
+      </c>
+      <c r="D3" s="6">
+        <v>120</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="6">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="6">
+        <v>65</v>
+      </c>
+      <c r="D4" s="6">
+        <v>70</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="6">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="6">
+        <v>55</v>
+      </c>
+      <c r="D5" s="6">
+        <v>83</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="6">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="6">
+        <v>53</v>
+      </c>
+      <c r="D6" s="6">
+        <v>85</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="6">
+        <v>18.8</v>
+      </c>
+      <c r="D7" s="6">
+        <v>260</v>
+      </c>
+      <c r="F7" s="6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="6">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="D8" s="6">
+        <v>130</v>
+      </c>
+      <c r="F8" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="14">
+        <v>420</v>
+      </c>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="6">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A8:B8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24794DDA-4385-44EC-8AD6-9CEA567538CF}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="V36" sqref="V36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U35" sqref="U35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add jmeter project for xAPI load test
</commit_message>
<xml_diff>
--- a/Reports/3.0.0-2020_05_06.xlsx
+++ b/Reports/3.0.0-2020_05_06.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\VirtoCommerce\vc-benchmark\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF001BA6-C74D-4053-A9BE-28E0D381D179}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D1A8A4C-ADC8-4602-B9EB-BF2A2F4EFA7F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -569,7 +569,7 @@
                   <c:v>350</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>200</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1753,12 +1753,21 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Maintenability</a:t>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Other p</a:t>
             </a:r>
             <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>erformance related metrics tests</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> tests </a:t>
+              <a:t>Comparative with 2.x version </a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1787,17 +1796,14 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'3.0.0 - 2020-06-05'!$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Full indexation time (sec)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>3.0</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+          </c:dPt>
           <c:dLbls>
             <c:spPr>
               <a:noFill/>
@@ -1822,12 +1828,15 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>'3.0.0 - 2020-06-05'!$C$9</c:f>
+              <c:f>'3.0.0 - 2020-06-05'!$C$9:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1839,20 +1848,18 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="3"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'3.0.0 - 2020-06-05'!$A$10</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Platform restart time (sec)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>2.0</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr/>
+          </c:dPt>
           <c:dLbls>
             <c:spPr>
               <a:noFill/>
@@ -1877,19 +1884,22 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>'3.0.0 - 2020-06-05'!$C$10</c:f>
+              <c:f>'2.13.63 - 2020-06-05'!$C$9:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-3EDD-4D75-B2C7-4E9E1819821E}"/>
+              <c16:uniqueId val="{00000010-3EDD-4D75-B2C7-4E9E1819821E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3627,7 +3637,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3744,7 +3754,7 @@
         <v>24.1</v>
       </c>
       <c r="D8" s="6">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="F8" s="6">
         <v>70</v>
@@ -3781,7 +3791,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3933,8 +3943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24794DDA-4385-44EC-8AD6-9CEA567538CF}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U35" sqref="U35"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="V31" sqref="V31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>